<commit_message>
selected data with the different diseases and age requirements
</commit_message>
<xml_diff>
--- a/3rdNF.xlsx
+++ b/3rdNF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasoncalle/Desktop/Books/Backend/SQL/Project4MedicalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF3F7EE-4321-224E-8BDC-82706E1C6786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA65801-C76C-C244-8AA1-937A771C53BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="3020" windowWidth="27640" windowHeight="16940" xr2:uid="{3F1DFE5F-97A7-C146-B8E9-1A03AB85E2F4}"/>
+    <workbookView xWindow="11080" yWindow="5480" windowWidth="27640" windowHeight="16940" xr2:uid="{3F1DFE5F-97A7-C146-B8E9-1A03AB85E2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
   <si>
     <t>Customer_id</t>
   </si>
@@ -243,30 +243,12 @@
     <t>Generate a list of patients with name, ordered by age, showing which is the most common disease amongst Senior citiezens</t>
   </si>
   <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
     <t>PK</t>
   </si>
   <si>
-    <t>Attribute</t>
-  </si>
-  <si>
     <t>Zipcode</t>
   </si>
   <si>
-    <t>A city can have multiple zipcodes</t>
-  </si>
-  <si>
-    <t>Table 2: State-City as the state can have different cities</t>
-  </si>
-  <si>
-    <t>Table 3</t>
-  </si>
-  <si>
-    <t>Table4</t>
-  </si>
-  <si>
     <t>employment</t>
   </si>
   <si>
@@ -291,9 +273,6 @@
     <t>I think these are temporary tables</t>
   </si>
   <si>
-    <t>Table 1: Overview</t>
-  </si>
-  <si>
     <t>Health:1</t>
   </si>
   <si>
@@ -343,6 +322,21 @@
   </si>
   <si>
     <t>Health 1</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>Table 1: CUSTOMER_INFO</t>
+  </si>
+  <si>
+    <t>Table 2: CUSTOMER_ADDRESS</t>
+  </si>
+  <si>
+    <t>PK and FK</t>
+  </si>
+  <si>
+    <t>For now we will not break this down but we may have to</t>
   </si>
 </sst>
 </file>
@@ -735,22 +729,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90516578-61E7-254C-A41D-3A765DCF8C07}">
-  <dimension ref="A1:Z44"/>
+  <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:E32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="135" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="24.5" customWidth="1"/>
-    <col min="8" max="8" width="27.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20.5" customWidth="1"/>
-    <col min="10" max="10" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
     <col min="12" max="12" width="16.1640625" customWidth="1"/>
     <col min="14" max="14" width="22" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
@@ -1160,66 +1154,66 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="O6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="P6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="R6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="U6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" t="s">
+        <v>82</v>
+      </c>
+      <c r="O8" t="s">
+        <v>83</v>
+      </c>
+      <c r="P8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>85</v>
+      </c>
+      <c r="R8" t="s">
         <v>86</v>
       </c>
-      <c r="L8" t="s">
+      <c r="S8" t="s">
         <v>87</v>
       </c>
-      <c r="M8" t="s">
+      <c r="T8" t="s">
         <v>88</v>
       </c>
-      <c r="N8" t="s">
+      <c r="U8" t="s">
         <v>89</v>
       </c>
-      <c r="O8" t="s">
+      <c r="V8" t="s">
         <v>90</v>
       </c>
-      <c r="P8" t="s">
+      <c r="W8" t="s">
         <v>91</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="X8" t="s">
         <v>92</v>
       </c>
-      <c r="R8" t="s">
+      <c r="Y8" t="s">
         <v>93</v>
       </c>
-      <c r="S8" t="s">
+      <c r="Z8" t="s">
         <v>94</v>
-      </c>
-      <c r="T8" t="s">
-        <v>95</v>
-      </c>
-      <c r="U8" t="s">
-        <v>96</v>
-      </c>
-      <c r="V8" t="s">
-        <v>97</v>
-      </c>
-      <c r="W8" t="s">
-        <v>98</v>
-      </c>
-      <c r="X8" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -1232,626 +1226,589 @@
         <v>60</v>
       </c>
     </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="F16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="H17" s="4"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
-        <v>19610</v>
+      <c r="B18" t="s">
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J18" s="5"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="B19">
-        <v>66080</v>
+      <c r="B19" t="s">
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="B20">
-        <v>45653</v>
+      <c r="B20" t="s">
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" t="s">
+        <v>19</v>
+      </c>
+      <c r="K34" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" t="s">
+        <v>23</v>
+      </c>
+      <c r="O34" t="s">
+        <v>24</v>
+      </c>
+      <c r="P34" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="2">
+        <v>79</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" t="s">
+        <v>38</v>
+      </c>
+      <c r="H35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" t="s">
+        <v>36</v>
+      </c>
+      <c r="J35" t="s">
+        <v>36</v>
+      </c>
+      <c r="K35" t="s">
+        <v>37</v>
+      </c>
+      <c r="L35" t="s">
+        <v>36</v>
+      </c>
+      <c r="M35" t="s">
+        <v>36</v>
+      </c>
+      <c r="N35" t="s">
+        <v>36</v>
+      </c>
+      <c r="O35" t="s">
+        <v>37</v>
+      </c>
+      <c r="P35" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="2">
+        <v>58</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36" t="s">
+        <v>37</v>
+      </c>
+      <c r="L36" t="s">
+        <v>37</v>
+      </c>
+      <c r="M36" t="s">
+        <v>37</v>
+      </c>
+      <c r="N36" t="s">
+        <v>37</v>
+      </c>
+      <c r="O36" t="s">
+        <v>36</v>
+      </c>
+      <c r="P36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="2">
+        <v>61</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I37" t="s">
+        <v>37</v>
+      </c>
+      <c r="J37" t="s">
+        <v>36</v>
+      </c>
+      <c r="K37" t="s">
+        <v>37</v>
+      </c>
+      <c r="L37" t="s">
+        <v>37</v>
+      </c>
+      <c r="M37" t="s">
+        <v>37</v>
+      </c>
+      <c r="N37" t="s">
+        <v>37</v>
+      </c>
+      <c r="O37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P37" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
         <v>3</v>
       </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="V25" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L26" t="s">
-        <v>15</v>
-      </c>
-      <c r="M26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" t="s">
-        <v>17</v>
-      </c>
-      <c r="O26" t="s">
-        <v>18</v>
-      </c>
-      <c r="P26" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>20</v>
-      </c>
-      <c r="R26" t="s">
-        <v>21</v>
-      </c>
-      <c r="S26" t="s">
-        <v>22</v>
-      </c>
-      <c r="T26" t="s">
-        <v>23</v>
-      </c>
-      <c r="U26" t="s">
-        <v>24</v>
-      </c>
-      <c r="V26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" t="s">
-        <v>34</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I27" s="2">
-        <v>79</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" t="s">
-        <v>37</v>
-      </c>
-      <c r="M27" t="s">
-        <v>38</v>
-      </c>
-      <c r="N27" t="s">
-        <v>37</v>
-      </c>
-      <c r="O27" t="s">
-        <v>36</v>
-      </c>
-      <c r="P27" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>37</v>
-      </c>
-      <c r="R27" t="s">
-        <v>36</v>
-      </c>
-      <c r="S27" t="s">
-        <v>36</v>
-      </c>
-      <c r="T27" t="s">
-        <v>36</v>
-      </c>
-      <c r="U27" t="s">
-        <v>37</v>
-      </c>
-      <c r="V27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" t="s">
-        <v>34</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I28" s="2">
-        <v>58</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L28" t="s">
-        <v>37</v>
-      </c>
-      <c r="M28" t="s">
-        <v>49</v>
-      </c>
-      <c r="N28" t="s">
-        <v>36</v>
-      </c>
-      <c r="O28" t="s">
-        <v>37</v>
-      </c>
-      <c r="P28" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>37</v>
-      </c>
-      <c r="R28" t="s">
-        <v>37</v>
-      </c>
-      <c r="S28" t="s">
-        <v>37</v>
-      </c>
-      <c r="T28" t="s">
-        <v>37</v>
-      </c>
-      <c r="U28" t="s">
-        <v>36</v>
-      </c>
-      <c r="V28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="F29" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G29" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I29" s="2">
-        <v>61</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L29" t="s">
-        <v>37</v>
-      </c>
-      <c r="M29" t="s">
-        <v>38</v>
-      </c>
-      <c r="N29" t="s">
-        <v>36</v>
-      </c>
-      <c r="O29" t="s">
-        <v>37</v>
-      </c>
-      <c r="P29" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>37</v>
-      </c>
-      <c r="R29" t="s">
-        <v>37</v>
-      </c>
-      <c r="S29" t="s">
-        <v>37</v>
-      </c>
-      <c r="T29" t="s">
-        <v>37</v>
-      </c>
-      <c r="U29" t="s">
-        <v>37</v>
-      </c>
-      <c r="V29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F36" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="2">
-        <v>1</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F39" s="2">
-        <v>2</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F40" s="2">
-        <v>3</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F43" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
returning customer_id within subqueries
</commit_message>
<xml_diff>
--- a/3rdNF.xlsx
+++ b/3rdNF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasoncalle/Desktop/Books/Backend/SQL/Project4MedicalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA65801-C76C-C244-8AA1-937A771C53BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C7A901-E1C4-6C49-BEEA-FAD9D78B6F4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11080" yWindow="5480" windowWidth="27640" windowHeight="16940" xr2:uid="{3F1DFE5F-97A7-C146-B8E9-1A03AB85E2F4}"/>
+    <workbookView xWindow="10760" yWindow="4160" windowWidth="27640" windowHeight="16940" xr2:uid="{3F1DFE5F-97A7-C146-B8E9-1A03AB85E2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90516578-61E7-254C-A41D-3A765DCF8C07}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="135" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Stored procedure that returns an output value
</commit_message>
<xml_diff>
--- a/3rdNF.xlsx
+++ b/3rdNF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasoncalle/Desktop/Books/Backend/SQL/Project4MedicalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C7A901-E1C4-6C49-BEEA-FAD9D78B6F4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E973D3-7346-F843-AE64-43B161526689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="4160" windowWidth="27640" windowHeight="16940" xr2:uid="{3F1DFE5F-97A7-C146-B8E9-1A03AB85E2F4}"/>
   </bookViews>
@@ -731,13 +731,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90516578-61E7-254C-A41D-3A765DCF8C07}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="135" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>

</xml_diff>

<commit_message>
completed 11 and started 12
</commit_message>
<xml_diff>
--- a/3rdNF.xlsx
+++ b/3rdNF.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasoncalle/Desktop/Books/Backend/SQL/Project4MedicalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E973D3-7346-F843-AE64-43B161526689}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DF133C-C233-614E-8444-D00BAE2F13DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="4160" windowWidth="27640" windowHeight="16940" xr2:uid="{3F1DFE5F-97A7-C146-B8E9-1A03AB85E2F4}"/>
+    <workbookView xWindow="320" yWindow="2980" windowWidth="27640" windowHeight="16940" xr2:uid="{3F1DFE5F-97A7-C146-B8E9-1A03AB85E2F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="128">
   <si>
     <t>Customer_id</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Table 4: Customer_id and Job</t>
   </si>
   <si>
-    <t>Table 5: Customer's Health</t>
-  </si>
-  <si>
     <t xml:space="preserve">Table 6: Caridac_Patients </t>
   </si>
   <si>
@@ -337,13 +334,97 @@
   </si>
   <si>
     <t>For now we will not break this down but we may have to</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>FK connecting the customer with their conditions</t>
+  </si>
+  <si>
+    <t>Table 1: Customer's Health</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -379,13 +460,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -400,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,6 +507,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -731,14 +830,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90516578-61E7-254C-A41D-3A765DCF8C07}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="135" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="7" width="13" customWidth="1"/>
@@ -1154,70 +1254,150 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="O6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U6" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" t="s">
+        <v>82</v>
+      </c>
+      <c r="P7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>84</v>
+      </c>
+      <c r="R7" t="s">
+        <v>85</v>
+      </c>
+      <c r="S7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T7" t="s">
+        <v>87</v>
+      </c>
+      <c r="U7" t="s">
+        <v>88</v>
+      </c>
+      <c r="V7" t="s">
+        <v>89</v>
+      </c>
+      <c r="W7" t="s">
+        <v>90</v>
+      </c>
+      <c r="X7" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" t="s">
+        <v>107</v>
+      </c>
       <c r="I8" t="s">
-        <v>79</v>
+        <v>108</v>
+      </c>
+      <c r="J8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" t="s">
+        <v>110</v>
       </c>
       <c r="L8" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="M8" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="N8" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="O8" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="P8" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="Q8" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="R8" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="S8" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="T8" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="U8" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="V8" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="W8" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="X8" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="Y8" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="Z8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1227,55 +1407,197 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="H13" t="s">
+      <c r="T13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="M14" t="s">
+        <v>119</v>
+      </c>
+      <c r="N14" t="s">
+        <v>120</v>
+      </c>
+      <c r="O14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P14" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>123</v>
+      </c>
+      <c r="R14" t="s">
+        <v>124</v>
+      </c>
+      <c r="S14" t="s">
+        <v>125</v>
+      </c>
+      <c r="T14" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="C15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="D16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="T17" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1285,17 +1607,59 @@
       <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="2">
+        <v>79</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>36</v>
+      </c>
+      <c r="R18" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" t="s">
+        <v>36</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1305,17 +1669,59 @@
       <c r="C19" t="s">
         <v>45</v>
       </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="2">
+        <v>58</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" t="s">
+        <v>36</v>
+      </c>
+      <c r="L19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O19" t="s">
+        <v>37</v>
+      </c>
+      <c r="P19" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>37</v>
+      </c>
+      <c r="R19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S19" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1325,394 +1731,270 @@
       <c r="C20" t="s">
         <v>55</v>
       </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="2">
+        <v>61</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" t="s">
+        <v>36</v>
+      </c>
+      <c r="N20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>37</v>
+      </c>
+      <c r="R20" t="s">
+        <v>37</v>
+      </c>
+      <c r="S20" t="s">
+        <v>37</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="I28" s="4"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>2</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>5</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E29" t="s">
         <v>4</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F29" t="s">
         <v>6</v>
       </c>
-      <c r="G26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="G27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C29" s="3"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="G29" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" t="s">
-        <v>19</v>
-      </c>
-      <c r="K34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L34" t="s">
-        <v>21</v>
-      </c>
-      <c r="M34" t="s">
-        <v>22</v>
-      </c>
-      <c r="N34" t="s">
-        <v>23</v>
-      </c>
-      <c r="O34" t="s">
-        <v>24</v>
-      </c>
-      <c r="P34" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q34" s="2" t="s">
+      <c r="I29" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="2">
-        <v>79</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F35" t="s">
-        <v>37</v>
-      </c>
-      <c r="G35" t="s">
-        <v>38</v>
-      </c>
-      <c r="H35" t="s">
-        <v>37</v>
-      </c>
-      <c r="I35" t="s">
-        <v>36</v>
-      </c>
-      <c r="J35" t="s">
-        <v>36</v>
-      </c>
-      <c r="K35" t="s">
-        <v>37</v>
-      </c>
-      <c r="L35" t="s">
-        <v>36</v>
-      </c>
-      <c r="M35" t="s">
-        <v>36</v>
-      </c>
-      <c r="N35" t="s">
-        <v>36</v>
-      </c>
-      <c r="O35" t="s">
-        <v>37</v>
-      </c>
-      <c r="P35" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q35" s="2" t="s">
+      <c r="J29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>19610</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <v>15439</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="2">
+      <c r="I30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" t="s">
-        <v>37</v>
-      </c>
-      <c r="G36" t="s">
-        <v>49</v>
-      </c>
-      <c r="H36" t="s">
-        <v>36</v>
-      </c>
-      <c r="I36" t="s">
-        <v>37</v>
-      </c>
-      <c r="J36" t="s">
-        <v>37</v>
-      </c>
-      <c r="K36" t="s">
-        <v>37</v>
-      </c>
-      <c r="L36" t="s">
-        <v>37</v>
-      </c>
-      <c r="M36" t="s">
-        <v>37</v>
-      </c>
-      <c r="N36" t="s">
-        <v>37</v>
-      </c>
-      <c r="O36" t="s">
-        <v>36</v>
-      </c>
-      <c r="P36" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q36" s="2" t="s">
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>66080</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31">
+        <v>922</v>
+      </c>
+      <c r="F31" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="2">
-        <v>61</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F37" t="s">
-        <v>37</v>
-      </c>
-      <c r="G37" t="s">
-        <v>38</v>
-      </c>
-      <c r="H37" t="s">
-        <v>36</v>
-      </c>
-      <c r="I37" t="s">
-        <v>37</v>
-      </c>
-      <c r="J37" t="s">
-        <v>36</v>
-      </c>
-      <c r="K37" t="s">
-        <v>37</v>
-      </c>
-      <c r="L37" t="s">
-        <v>37</v>
-      </c>
-      <c r="M37" t="s">
-        <v>37</v>
-      </c>
-      <c r="N37" t="s">
-        <v>37</v>
-      </c>
-      <c r="O37" t="s">
-        <v>37</v>
-      </c>
-      <c r="P37" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q37" s="2" t="s">
+      <c r="I31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>45653</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32">
+        <v>3782</v>
+      </c>
+      <c r="F32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>14</v>
@@ -1727,7 +2009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>1</v>
       </c>
@@ -1747,7 +2029,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>2</v>
       </c>
@@ -1767,7 +2049,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>3</v>
       </c>
@@ -1803,7 +2085,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>

</xml_diff>